<commit_message>
etc: changed first pilot tagging data
</commit_message>
<xml_diff>
--- a/tagging_data/pilot_tagging.xlsx
+++ b/tagging_data/pilot_tagging.xlsx
@@ -9,7 +9,7 @@
     <sheet state="visible" name="재학" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="성진" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="나연" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Metric" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Main" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="657">
   <si>
     <t>Index</t>
   </si>
@@ -1855,21 +1855,21 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <color theme="4"/>
+      </rPr>
+      <t>아제르바이잔</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">의 월경지 </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
         <color theme="5"/>
-      </rPr>
-      <t>아제르바이잔</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">의 월경지 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="4"/>
       </rPr>
       <t>나히체반 자치 공화국</t>
     </r>
@@ -21744,21 +21744,6 @@
       </rPr>
       <t>에 맞써 싸우는 선도적인 군사 중 하나이다.</t>
     </r>
-  </si>
-  <si>
-    <t>member1</t>
-  </si>
-  <si>
-    <t>member2</t>
-  </si>
-  <si>
-    <t>member3</t>
-  </si>
-  <si>
-    <t>member4</t>
-  </si>
-  <si>
-    <t>member5</t>
   </si>
 </sst>
 </file>
@@ -22386,12 +22371,12 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="7.13"/>
     <col customWidth="1" min="3" max="3" width="84.13"/>
-    <col customWidth="1" min="4" max="4" width="22.5"/>
-    <col customWidth="1" min="5" max="5" width="26.63"/>
+    <col customWidth="1" min="4" max="4" width="17.88"/>
+    <col customWidth="1" min="5" max="5" width="18.0"/>
     <col customWidth="1" min="6" max="6" width="18.25"/>
     <col customWidth="1" min="7" max="7" width="19.13"/>
     <col customWidth="1" min="8" max="8" width="18.63"/>
-    <col customWidth="1" min="9" max="9" width="15.75"/>
+    <col customWidth="1" min="9" max="9" width="17.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -22472,7 +22457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="B4" s="7">
         <v>3.0</v>
       </c>
@@ -22498,7 +22483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="B5" s="7">
         <v>4.0</v>
       </c>
@@ -22524,7 +22509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="B6" s="7">
         <v>5.0</v>
       </c>
@@ -22548,7 +22533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="B7" s="7">
         <v>6.0</v>
       </c>
@@ -22574,7 +22559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" ht="24.75" customHeight="1">
+    <row r="8" ht="24.75" hidden="1" customHeight="1">
       <c r="B8" s="7">
         <v>7.0</v>
       </c>
@@ -22600,7 +22585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="B9" s="7">
         <v>8.0</v>
       </c>
@@ -22626,7 +22611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="s">
         <v>24</v>
@@ -22640,7 +22625,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="B11" s="7">
         <v>9.0</v>
       </c>
@@ -22664,7 +22649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="B12" s="7">
         <v>10.0</v>
       </c>
@@ -22690,7 +22675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="B13" s="7">
         <v>11.0</v>
       </c>
@@ -22716,7 +22701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="B14" s="7">
         <v>12.0</v>
       </c>
@@ -22740,7 +22725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="B15" s="7">
         <v>13.0</v>
       </c>
@@ -22764,7 +22749,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="B16" s="7">
         <v>14.0</v>
       </c>
@@ -22788,7 +22773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="B17" s="7">
         <v>15.0</v>
       </c>
@@ -22812,7 +22797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="B18" s="7">
         <v>16.0</v>
       </c>
@@ -22838,7 +22823,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="B19" s="7">
         <v>17.0</v>
       </c>
@@ -22864,7 +22849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="B20" s="7">
         <v>18.0</v>
       </c>
@@ -22888,7 +22873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="B21" s="7">
         <v>19.0</v>
       </c>
@@ -22995,7 +22980,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="B25" s="17">
         <v>23.0</v>
       </c>
@@ -23019,7 +23004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="B26" s="17">
         <v>24.0</v>
       </c>
@@ -23043,7 +23028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="B27" s="17">
         <v>25.0</v>
       </c>
@@ -23067,7 +23052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="B28" s="17">
         <v>26.0</v>
       </c>
@@ -23091,7 +23076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="B29" s="17">
         <v>27.0</v>
       </c>
@@ -23117,7 +23102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="B30" s="17">
         <v>28.0</v>
       </c>
@@ -23141,7 +23126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="B31" s="17">
         <v>29.0</v>
       </c>
@@ -23165,7 +23150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="B32" s="17">
         <v>30.0</v>
       </c>
@@ -23189,7 +23174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="B33" s="17">
         <v>31.0</v>
       </c>
@@ -23213,7 +23198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="B34" s="17">
         <v>32.0</v>
       </c>
@@ -23239,7 +23224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="B35" s="17">
         <v>33.0</v>
       </c>
@@ -23263,7 +23248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1">
       <c r="B36" s="17">
         <v>34.0</v>
       </c>
@@ -23289,7 +23274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="1">
       <c r="B37" s="17">
         <v>35.0</v>
       </c>
@@ -23315,7 +23300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="B38" s="17">
         <v>36.0</v>
       </c>
@@ -23341,7 +23326,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="B39" s="17">
         <v>37.0</v>
       </c>
@@ -23365,7 +23350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="B40" s="17">
         <v>38.0</v>
       </c>
@@ -23391,7 +23376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="1">
       <c r="B41" s="17">
         <v>39.0</v>
       </c>
@@ -23494,7 +23479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c r="B45" s="20">
         <v>43.0</v>
       </c>
@@ -23518,7 +23503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1">
       <c r="B46" s="20">
         <v>44.0</v>
       </c>
@@ -23542,7 +23527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c r="B47" s="20">
         <v>45.0</v>
       </c>
@@ -23568,7 +23553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="B48" s="20">
         <v>46.0</v>
       </c>
@@ -23592,7 +23577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="B49" s="20">
         <v>47.0</v>
       </c>
@@ -23616,7 +23601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="1">
       <c r="B50" s="20">
         <v>48.0</v>
       </c>
@@ -23642,7 +23627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1">
       <c r="B51" s="20">
         <v>49.0</v>
       </c>
@@ -23668,7 +23653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="1">
       <c r="B52" s="20">
         <v>50.0</v>
       </c>
@@ -23694,7 +23679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1">
       <c r="B53" s="20">
         <v>51.0</v>
       </c>
@@ -23720,7 +23705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1">
       <c r="B54" s="20">
         <v>52.0</v>
       </c>
@@ -23744,7 +23729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="B55" s="20">
         <v>53.0</v>
       </c>
@@ -23768,7 +23753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c r="B56" s="20">
         <v>54.0</v>
       </c>
@@ -23792,7 +23777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="B57" s="20">
         <v>55.0</v>
       </c>
@@ -23818,7 +23803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c r="B58" s="20">
         <v>56.0</v>
       </c>
@@ -23844,7 +23829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c r="B59" s="20">
         <v>57.0</v>
       </c>
@@ -23870,7 +23855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="B60" s="20">
         <v>58.0</v>
       </c>
@@ -23896,7 +23881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c r="B61" s="20">
         <v>59.0</v>
       </c>
@@ -23997,7 +23982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="1">
       <c r="B65" s="24">
         <v>63.0</v>
       </c>
@@ -24021,7 +24006,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c r="B66" s="24">
         <v>64.0</v>
       </c>
@@ -24045,7 +24030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c r="B67" s="24">
         <v>65.0</v>
       </c>
@@ -24061,7 +24046,7 @@
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
     </row>
-    <row r="68">
+    <row r="68" hidden="1">
       <c r="B68" s="24">
         <v>66.0</v>
       </c>
@@ -24085,7 +24070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="1">
       <c r="B69" s="24">
         <v>67.0</v>
       </c>
@@ -24111,7 +24096,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="1">
       <c r="B70" s="24">
         <v>68.0</v>
       </c>
@@ -24135,7 +24120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c r="B71" s="24">
         <v>69.0</v>
       </c>
@@ -24159,7 +24144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="1">
       <c r="B72" s="24">
         <v>70.0</v>
       </c>
@@ -24183,7 +24168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c r="B73" s="24">
         <v>71.0</v>
       </c>
@@ -24207,7 +24192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c r="B74" s="24">
         <v>72.0</v>
       </c>
@@ -24233,7 +24218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c r="B75" s="24">
         <v>73.0</v>
       </c>
@@ -24257,7 +24242,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c r="B76" s="24">
         <v>74.0</v>
       </c>
@@ -24281,7 +24266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c r="B77" s="24">
         <v>75.0</v>
       </c>
@@ -24307,7 +24292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c r="B78" s="24">
         <v>76.0</v>
       </c>
@@ -24331,7 +24316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c r="B79" s="24">
         <v>77.0</v>
       </c>
@@ -24355,7 +24340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c r="B80" s="24">
         <v>78.0</v>
       </c>
@@ -24381,7 +24366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="1">
       <c r="B81" s="24">
         <v>79.0</v>
       </c>
@@ -24486,7 +24471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c r="B85" s="7">
         <v>83.0</v>
       </c>
@@ -24512,7 +24497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c r="B86" s="7">
         <v>84.0</v>
       </c>
@@ -24536,7 +24521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c r="B87" s="7">
         <v>85.0</v>
       </c>
@@ -24560,7 +24545,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c r="B88" s="7">
         <v>86.0</v>
       </c>
@@ -24586,7 +24571,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c r="B89" s="7">
         <v>87.0</v>
       </c>
@@ -24610,7 +24595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c r="B90" s="7">
         <v>88.0</v>
       </c>
@@ -24634,7 +24619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="1">
       <c r="B91" s="7">
         <v>89.0</v>
       </c>
@@ -24658,7 +24643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c r="B92" s="7">
         <v>90.0</v>
       </c>
@@ -24684,7 +24669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c r="B93" s="7">
         <v>91.0</v>
       </c>
@@ -24708,7 +24693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c r="B94" s="7">
         <v>92.0</v>
       </c>
@@ -24734,7 +24719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="1">
       <c r="B95" s="7">
         <v>93.0</v>
       </c>
@@ -24760,7 +24745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c r="B96" s="7">
         <v>94.0</v>
       </c>
@@ -24786,7 +24771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c r="B97" s="7">
         <v>95.0</v>
       </c>
@@ -24812,7 +24797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c r="B98" s="7">
         <v>96.0</v>
       </c>
@@ -24838,7 +24823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c r="B99" s="7">
         <v>97.0</v>
       </c>
@@ -24862,7 +24847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c r="B100" s="7">
         <v>98.0</v>
       </c>
@@ -24886,7 +24871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1">
       <c r="B101" s="7">
         <v>99.0</v>
       </c>
@@ -57060,19 +57045,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>657</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>658</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>659</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>660</v>
+        <v>6</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>661</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>

</xml_diff>